<commit_message>
Addressed QA for example_config file
</commit_message>
<xml_diff>
--- a/14-2-1/Example_Input/ukbi2022-ds-c1.xlsx
+++ b/14-2-1/Example_Input/ukbi2022-ds-c1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3D0EA2-B98A-4707-B24F-FEF29393751B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42738D2-210D-4867-AAD4-73A033350174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D77" sqref="A75:D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1741,50 +1741,26 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="10">
-        <v>2020</v>
-      </c>
-      <c r="B75" s="11">
-        <v>6.7930987426999998</v>
-      </c>
-      <c r="C75" s="11">
-        <v>33.821657997800003</v>
-      </c>
-      <c r="D75" s="11">
-        <v>40.614756740499999</v>
-      </c>
+      <c r="A75" s="10"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
     </row>
     <row r="76" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="10">
-        <v>2021</v>
-      </c>
-      <c r="B76" s="14">
-        <v>6.7916245691999988</v>
-      </c>
-      <c r="C76" s="15">
-        <v>33.823470902699995</v>
-      </c>
-      <c r="D76" s="14">
-        <v>40.615095471899991</v>
-      </c>
+      <c r="A76" s="10"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="14"/>
       <c r="F76" s="4"/>
       <c r="G76" s="5"/>
       <c r="H76" s="6"/>
       <c r="I76" s="5"/>
     </row>
     <row r="77" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="10">
-        <v>2022</v>
-      </c>
-      <c r="B77" s="14">
-        <v>6.7922804960999992</v>
-      </c>
-      <c r="C77" s="15">
-        <v>33.823470902699995</v>
-      </c>
-      <c r="D77" s="14">
-        <v>40.615751398799993</v>
-      </c>
+      <c r="A77" s="10"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="14"/>
       <c r="F77" s="4"/>
       <c r="G77" s="5"/>
       <c r="H77" s="6"/>

</xml_diff>

<commit_message>
Addressed ReadMe file QA
</commit_message>
<xml_diff>
--- a/14-2-1/Example_Input/ukbi2022-ds-c1.xlsx
+++ b/14-2-1/Example_Input/ukbi2022-ds-c1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42738D2-210D-4867-AAD4-73A033350174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20564976-AA72-4590-AE2E-49E5D480F8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D77" sqref="A75:D77"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1741,26 +1741,50 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="10"/>
-      <c r="B75" s="11"/>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
+      <c r="A75" s="10">
+        <v>2020</v>
+      </c>
+      <c r="B75" s="11">
+        <v>6.7930987426999998</v>
+      </c>
+      <c r="C75" s="11">
+        <v>33.821657997800003</v>
+      </c>
+      <c r="D75" s="11">
+        <v>40.614756740499999</v>
+      </c>
     </row>
     <row r="76" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="10"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="15"/>
-      <c r="D76" s="14"/>
+      <c r="A76" s="10">
+        <v>2021</v>
+      </c>
+      <c r="B76" s="14">
+        <v>6.7916245691999988</v>
+      </c>
+      <c r="C76" s="15">
+        <v>33.823470902699995</v>
+      </c>
+      <c r="D76" s="14">
+        <v>40.615095471899991</v>
+      </c>
       <c r="F76" s="4"/>
       <c r="G76" s="5"/>
       <c r="H76" s="6"/>
       <c r="I76" s="5"/>
     </row>
     <row r="77" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="10"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="14"/>
+      <c r="A77" s="10">
+        <v>2022</v>
+      </c>
+      <c r="B77" s="14">
+        <v>6.7922804960999992</v>
+      </c>
+      <c r="C77" s="15">
+        <v>33.823470902699995</v>
+      </c>
+      <c r="D77" s="14">
+        <v>40.615751398799993</v>
+      </c>
       <c r="F77" s="4"/>
       <c r="G77" s="5"/>
       <c r="H77" s="6"/>

</xml_diff>